<commit_message>
fix: salary import to all
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-salary-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-salary-template.xlsx
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lambert\accupay\AccuPay\ImportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="h8nPxDaFOl90V67rBlj+f3z5aPJCqTexv2ykK/S3t1BAKEd0Tn7EBousbJJvKrR2fUyayFCPmXhAUqwXJNTEuQ==" workbookSaltValue="d3MH/Po41O59BKIvRDPvew==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
@@ -187,14 +188,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,10 +492,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="20"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -507,17 +508,17 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -636,18 +637,19 @@
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="89.7109375" style="12" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" style="13" customWidth="1"/>
     <col min="3" max="4" width="20.7109375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="0" style="21" hidden="1" customWidth="1"/>
-    <col min="6" max="1023" width="9.140625" style="21"/>
-    <col min="1024" max="1025" width="11.5703125" style="21" customWidth="1"/>
-    <col min="1026" max="16384" width="9.140625" style="21"/>
+    <col min="5" max="5" width="15.5703125" style="19" hidden="1" customWidth="1"/>
+    <col min="6" max="1023" width="9.140625" style="19"/>
+    <col min="1024" max="1025" width="11.5703125" style="19" customWidth="1"/>
+    <col min="1026" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="18" customFormat="1">
@@ -666,11 +668,11 @@
       <c r="E1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="AMJ1" s="21"/>
+      <c r="AMJ1" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IqT4cDAd1cr0nWfH1LLVNE8MWhAfzkoG9wLUMcyTKuLsCGmp6IRbKNikcd19yCUxb3MHIlp3oWZJsM6MGju9BQ==" saltValue="/VeSQQF1FXoM3djmfdTMSw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="QimzrA4BEZ6k16CW9OnloTomijkibjroRzGVjRHKabkYgDgu4lyRTnMQSOM0QPenu7zHODGhuKXpnSWZ9DMShg==" saltValue="/T7vXjyytJjW43vO18XF3A==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>